<commit_message>
Add option --complete_perf + code cleaning
</commit_message>
<xml_diff>
--- a/ISPInput.xlsx
+++ b/ISPInput.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" tabRatio="744" firstSheet="3" activeTab="8" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" tabRatio="744" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bonnes pratiques" sheetId="1" state="visible" r:id="rId1"/>
@@ -258,7 +258,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="104">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1145,7 +1148,7 @@
   <autoFilter ref="A1:U34"/>
   <tableColumns count="21">
     <tableColumn id="1" name="_"/>
-    <tableColumn id="2" name="100mM" dataDxfId="102"/>
+    <tableColumn id="2" name="100mM" dataDxfId="103"/>
     <tableColumn id="3" name="200mM"/>
     <tableColumn id="4" name="400mM"/>
     <tableColumn id="5" name="800mM"/>
@@ -1163,8 +1166,8 @@
     <tableColumn id="17" name="javM"/>
     <tableColumn id="18" name="hammerM"/>
     <tableColumn id="19" name="discM"/>
-    <tableColumn id="20" name="4x100mM" dataDxfId="101"/>
-    <tableColumn id="21" name="4x400mM" dataDxfId="100"/>
+    <tableColumn id="20" name="4x100mM" dataDxfId="102"/>
+    <tableColumn id="21" name="4x400mM" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1175,7 +1178,7 @@
   <autoFilter ref="A1:T31"/>
   <tableColumns count="20">
     <tableColumn id="1" name="_"/>
-    <tableColumn id="2" name="100mW" dataDxfId="99"/>
+    <tableColumn id="2" name="100mW" dataDxfId="100"/>
     <tableColumn id="3" name="200mW"/>
     <tableColumn id="4" name="400mW"/>
     <tableColumn id="5" name="800mW"/>
@@ -1192,15 +1195,15 @@
     <tableColumn id="17" name="javW"/>
     <tableColumn id="18" name="hammerW"/>
     <tableColumn id="19" name="discW"/>
-    <tableColumn id="8" name="4x100mW" dataDxfId="98"/>
-    <tableColumn id="20" name="4x400mW" dataDxfId="97"/>
+    <tableColumn id="8" name="4x100mW" dataDxfId="99"/>
+    <tableColumn id="20" name="4x400mW" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau8" displayName="Tableau8" ref="A1:T31" headerRowCount="1" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau8" displayName="Tableau8" ref="A1:T31" headerRowCount="1" totalsRowShown="0" headerRowDxfId="97" headerRowBorderDxfId="96">
   <autoFilter ref="A1:T31"/>
   <tableColumns count="20">
     <tableColumn id="1" name="100mM"/>
@@ -1229,62 +1232,62 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau12" displayName="Tableau12" ref="A1:S31" headerRowCount="1" totalsRowShown="0" headerRowDxfId="94" dataDxfId="92" headerRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau12" displayName="Tableau12" ref="A1:S31" headerRowCount="1" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94">
   <autoFilter ref="A1:S31"/>
   <tableColumns count="19">
-    <tableColumn id="1" name="100mW" dataDxfId="91">
+    <tableColumn id="1" name="100mW" dataDxfId="92">
       <calculatedColumnFormula>ConflictsHelperW!C6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="200mW" dataDxfId="90">
+    <tableColumn id="2" name="200mW" dataDxfId="91">
       <calculatedColumnFormula>ConflictsHelperW!D6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="400mW" dataDxfId="89">
+    <tableColumn id="3" name="400mW" dataDxfId="90">
       <calculatedColumnFormula>ConflictsHelperW!E6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="800mW" dataDxfId="88">
+    <tableColumn id="4" name="800mW" dataDxfId="89">
       <calculatedColumnFormula>ConflictsHelperW!F6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="1500mW" dataDxfId="87">
+    <tableColumn id="5" name="1500mW" dataDxfId="88">
       <calculatedColumnFormula>ConflictsHelperW!G6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="3000mW" dataDxfId="86">
+    <tableColumn id="6" name="3000mW" dataDxfId="87">
       <calculatedColumnFormula>ConflictsHelperW!H6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="100mHW" dataDxfId="85">
+    <tableColumn id="7" name="100mHW" dataDxfId="86">
       <calculatedColumnFormula>ConflictsHelperW!I6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="400mHW" dataDxfId="84">
+    <tableColumn id="8" name="400mHW" dataDxfId="85">
       <calculatedColumnFormula>ConflictsHelperW!J6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="3000walkW" dataDxfId="83">
+    <tableColumn id="9" name="3000walkW" dataDxfId="84">
       <calculatedColumnFormula>ConflictsHelperW!K6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="longW" dataDxfId="82">
+    <tableColumn id="10" name="longW" dataDxfId="83">
       <calculatedColumnFormula>ConflictsHelperW!L6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="highW" dataDxfId="81">
+    <tableColumn id="11" name="highW" dataDxfId="82">
       <calculatedColumnFormula>ConflictsHelperW!M6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="tripleW" dataDxfId="80">
+    <tableColumn id="12" name="tripleW" dataDxfId="81">
       <calculatedColumnFormula>ConflictsHelperW!N6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="poleW" dataDxfId="79">
+    <tableColumn id="13" name="poleW" dataDxfId="80">
       <calculatedColumnFormula>ConflictsHelperW!O6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="shotW" dataDxfId="78">
+    <tableColumn id="14" name="shotW" dataDxfId="79">
       <calculatedColumnFormula>ConflictsHelperW!P6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="javW" dataDxfId="77">
+    <tableColumn id="15" name="javW" dataDxfId="78">
       <calculatedColumnFormula>ConflictsHelperW!Q6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="hammerW" dataDxfId="76">
+    <tableColumn id="16" name="hammerW" dataDxfId="77">
       <calculatedColumnFormula>ConflictsHelperW!R6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="discW" dataDxfId="75">
+    <tableColumn id="17" name="discW" dataDxfId="76">
       <calculatedColumnFormula>ConflictsHelperW!S6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="4x100mW" dataDxfId="74"/>
-    <tableColumn id="19" name="4x400mW" dataDxfId="73"/>
+    <tableColumn id="18" name="4x100mW" dataDxfId="75"/>
+    <tableColumn id="19" name="4x400mW" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1294,7 +1297,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau4" displayName="Tableau4" ref="A6:V35" headerRowCount="1" totalsRowShown="0">
   <autoFilter ref="A6:V35"/>
   <tableColumns count="22">
-    <tableColumn id="1" name="Debut" dataDxfId="72"/>
+    <tableColumn id="1" name="Debut" dataDxfId="73"/>
     <tableColumn id="20" name="Fin"/>
     <tableColumn id="2" name="100mM">
       <calculatedColumnFormula>IF(OR($A7&gt;B$3,B$2&gt;$B7),0,1)</calculatedColumnFormula>
@@ -1362,30 +1365,30 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau5" displayName="Tableau5" ref="A1:U3" headerRowCount="1" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau5" displayName="Tableau5" ref="A1:U3" headerRowCount="1" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:U3"/>
   <tableColumns count="21">
-    <tableColumn id="1" name="_" dataDxfId="69"/>
-    <tableColumn id="2" name="100mM" dataDxfId="68"/>
-    <tableColumn id="3" name="200mM" dataDxfId="67"/>
-    <tableColumn id="4" name="400mM" dataDxfId="66"/>
-    <tableColumn id="5" name="800mM" dataDxfId="65"/>
-    <tableColumn id="6" name="1500mM" dataDxfId="64"/>
-    <tableColumn id="7" name="3000mM" dataDxfId="63"/>
-    <tableColumn id="8" name="3000scM" dataDxfId="62"/>
-    <tableColumn id="9" name="110mHM" dataDxfId="61"/>
-    <tableColumn id="10" name="400mHM" dataDxfId="60"/>
-    <tableColumn id="11" name="5000walkM" dataDxfId="59"/>
-    <tableColumn id="12" name="longM" dataDxfId="58"/>
-    <tableColumn id="13" name="highM" dataDxfId="57"/>
-    <tableColumn id="14" name="tripleM" dataDxfId="56"/>
-    <tableColumn id="15" name="poleM" dataDxfId="55"/>
-    <tableColumn id="16" name="shotM" dataDxfId="54"/>
-    <tableColumn id="17" name="javM" dataDxfId="53"/>
-    <tableColumn id="18" name="hammerM" dataDxfId="52"/>
-    <tableColumn id="19" name="discM" dataDxfId="51"/>
-    <tableColumn id="20" name="4x100mM" dataDxfId="50"/>
-    <tableColumn id="21" name="4x400mM" dataDxfId="49"/>
+    <tableColumn id="1" name="_" dataDxfId="70"/>
+    <tableColumn id="2" name="100mM" dataDxfId="69"/>
+    <tableColumn id="3" name="200mM" dataDxfId="68"/>
+    <tableColumn id="4" name="400mM" dataDxfId="67"/>
+    <tableColumn id="5" name="800mM" dataDxfId="66"/>
+    <tableColumn id="6" name="1500mM" dataDxfId="65"/>
+    <tableColumn id="7" name="3000mM" dataDxfId="64"/>
+    <tableColumn id="8" name="3000scM" dataDxfId="63"/>
+    <tableColumn id="9" name="110mHM" dataDxfId="62"/>
+    <tableColumn id="10" name="400mHM" dataDxfId="61"/>
+    <tableColumn id="11" name="5000walkM" dataDxfId="60"/>
+    <tableColumn id="12" name="longM" dataDxfId="59"/>
+    <tableColumn id="13" name="highM" dataDxfId="58"/>
+    <tableColumn id="14" name="tripleM" dataDxfId="57"/>
+    <tableColumn id="15" name="poleM" dataDxfId="56"/>
+    <tableColumn id="16" name="shotM" dataDxfId="55"/>
+    <tableColumn id="17" name="javM" dataDxfId="54"/>
+    <tableColumn id="18" name="hammerM" dataDxfId="53"/>
+    <tableColumn id="19" name="discM" dataDxfId="52"/>
+    <tableColumn id="20" name="4x100mM" dataDxfId="51"/>
+    <tableColumn id="21" name="4x400mM" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1395,7 +1398,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau411" displayName="Tableau411" ref="A6:U35" headerRowCount="1" totalsRowShown="0">
   <autoFilter ref="A6:U35"/>
   <tableColumns count="21">
-    <tableColumn id="1" name="Debut" dataDxfId="48"/>
+    <tableColumn id="1" name="Debut" dataDxfId="49"/>
     <tableColumn id="20" name="Fin"/>
     <tableColumn id="2" name="100mW">
       <calculatedColumnFormula>IF(OR($A7&gt;B$3,B$2&gt;$B7),0,1)</calculatedColumnFormula>
@@ -1460,64 +1463,65 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau512" displayName="Tableau512" ref="A1:T3" headerRowCount="1" totalsRowShown="0" headerRowDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau512" displayName="Tableau512" ref="A1:T3" headerRowCount="1" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="A1:T3"/>
   <tableColumns count="20">
-    <tableColumn id="1" name="_" dataDxfId="46"/>
-    <tableColumn id="2" name="100mW" dataDxfId="45"/>
-    <tableColumn id="3" name="200mW" dataDxfId="44"/>
-    <tableColumn id="4" name="400mW" dataDxfId="43"/>
-    <tableColumn id="5" name="800mW" dataDxfId="42"/>
-    <tableColumn id="6" name="1500mW" dataDxfId="41"/>
-    <tableColumn id="7" name="3000mW" dataDxfId="40"/>
-    <tableColumn id="9" name="100mHW" dataDxfId="39"/>
-    <tableColumn id="10" name="400mHW" dataDxfId="38"/>
-    <tableColumn id="11" name="3000walkW" dataDxfId="37"/>
-    <tableColumn id="12" name="longW" dataDxfId="36"/>
-    <tableColumn id="13" name="highW" dataDxfId="35"/>
-    <tableColumn id="14" name="tripleW" dataDxfId="34"/>
-    <tableColumn id="15" name="poleW" dataDxfId="33"/>
-    <tableColumn id="16" name="shotW" dataDxfId="32"/>
-    <tableColumn id="17" name="javW" dataDxfId="31"/>
-    <tableColumn id="18" name="hammerW" dataDxfId="30"/>
-    <tableColumn id="19" name="discW" dataDxfId="29"/>
-    <tableColumn id="8" name="4x100mW" dataDxfId="28"/>
-    <tableColumn id="20" name="4x400mW" dataDxfId="27"/>
+    <tableColumn id="1" name="_" dataDxfId="47"/>
+    <tableColumn id="2" name="100mW" dataDxfId="46"/>
+    <tableColumn id="3" name="200mW" dataDxfId="45"/>
+    <tableColumn id="4" name="400mW" dataDxfId="44"/>
+    <tableColumn id="5" name="800mW" dataDxfId="43"/>
+    <tableColumn id="6" name="1500mW" dataDxfId="42"/>
+    <tableColumn id="7" name="3000mW" dataDxfId="41"/>
+    <tableColumn id="9" name="100mHW" dataDxfId="40"/>
+    <tableColumn id="10" name="400mHW" dataDxfId="39"/>
+    <tableColumn id="11" name="3000walkW" dataDxfId="38"/>
+    <tableColumn id="12" name="longW" dataDxfId="37"/>
+    <tableColumn id="13" name="highW" dataDxfId="36"/>
+    <tableColumn id="14" name="tripleW" dataDxfId="35"/>
+    <tableColumn id="15" name="poleW" dataDxfId="34"/>
+    <tableColumn id="16" name="shotW" dataDxfId="33"/>
+    <tableColumn id="17" name="javW" dataDxfId="32"/>
+    <tableColumn id="18" name="hammerW" dataDxfId="31"/>
+    <tableColumn id="19" name="discW" dataDxfId="30"/>
+    <tableColumn id="8" name="4x100mW" dataDxfId="29"/>
+    <tableColumn id="20" name="4x400mW" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau3" displayName="Tableau3" ref="A1:Z20" headerRowCount="1" totalsRowShown="0" headerRowDxfId="26">
-  <autoFilter ref="A1:Z20"/>
-  <tableColumns count="26">
-    <tableColumn id="1" name="NOM" dataDxfId="25"/>
-    <tableColumn id="2" name="Prenom" dataDxfId="24"/>
-    <tableColumn id="3" name="N° licence" dataDxfId="23"/>
-    <tableColumn id="4" name="Sexe" dataDxfId="22"/>
-    <tableColumn id="5" name="Colonne1" dataDxfId="21"/>
-    <tableColumn id="6" name="Colonne2" dataDxfId="20"/>
-    <tableColumn id="7" name="Colonne3" dataDxfId="19"/>
-    <tableColumn id="8" name="Colonne4" dataDxfId="18"/>
-    <tableColumn id="9" name="Colonne5" dataDxfId="17"/>
-    <tableColumn id="10" name="Colonne6" dataDxfId="16"/>
-    <tableColumn id="11" name="Colonne7" dataDxfId="15"/>
-    <tableColumn id="12" name="Colonne8" dataDxfId="14"/>
-    <tableColumn id="13" name="Colonne9" dataDxfId="13"/>
-    <tableColumn id="14" name="Colonne10" dataDxfId="12"/>
-    <tableColumn id="15" name="Colonne11" dataDxfId="11"/>
-    <tableColumn id="16" name="Colonne12" dataDxfId="10"/>
-    <tableColumn id="17" name="Colonne13" dataDxfId="9"/>
-    <tableColumn id="18" name="Colonne14" dataDxfId="8"/>
-    <tableColumn id="19" name="Colonne15" dataDxfId="7"/>
-    <tableColumn id="20" name="Colonne16" dataDxfId="6"/>
-    <tableColumn id="21" name="Colonne17" dataDxfId="5"/>
-    <tableColumn id="22" name="Colonne18" dataDxfId="4"/>
-    <tableColumn id="23" name="Colonne19" dataDxfId="3"/>
-    <tableColumn id="24" name="Colonne20" dataDxfId="2"/>
-    <tableColumn id="25" name="Colonne21" dataDxfId="1"/>
-    <tableColumn id="26" name="Colonne22" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau3" displayName="Tableau3" ref="A1:AA20" headerRowCount="1" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="A1:AA20"/>
+  <tableColumns count="27">
+    <tableColumn id="1" name="NOM" dataDxfId="26"/>
+    <tableColumn id="2" name="Prenom" dataDxfId="25"/>
+    <tableColumn id="3" name="N° licence" dataDxfId="24"/>
+    <tableColumn id="4" name="Sexe" dataDxfId="23"/>
+    <tableColumn id="5" name="Alias" dataDxfId="22"/>
+    <tableColumn id="6" name="Colonne2" dataDxfId="21"/>
+    <tableColumn id="7" name="Colonne3" dataDxfId="20"/>
+    <tableColumn id="8" name="Colonne4" dataDxfId="19"/>
+    <tableColumn id="9" name="Colonne5" dataDxfId="18"/>
+    <tableColumn id="10" name="Colonne6" dataDxfId="17"/>
+    <tableColumn id="11" name="Colonne7" dataDxfId="16"/>
+    <tableColumn id="12" name="Colonne8" dataDxfId="15"/>
+    <tableColumn id="13" name="Colonne9" dataDxfId="14"/>
+    <tableColumn id="14" name="Colonne10" dataDxfId="13"/>
+    <tableColumn id="15" name="Colonne11" dataDxfId="12"/>
+    <tableColumn id="16" name="Colonne12" dataDxfId="11"/>
+    <tableColumn id="17" name="Colonne13" dataDxfId="10"/>
+    <tableColumn id="18" name="Colonne14" dataDxfId="9"/>
+    <tableColumn id="19" name="Colonne15" dataDxfId="8"/>
+    <tableColumn id="20" name="Colonne16" dataDxfId="7"/>
+    <tableColumn id="21" name="Colonne17" dataDxfId="6"/>
+    <tableColumn id="22" name="Colonne18" dataDxfId="5"/>
+    <tableColumn id="23" name="Colonne19" dataDxfId="4"/>
+    <tableColumn id="24" name="Colonne20" dataDxfId="3"/>
+    <tableColumn id="25" name="Colonne21" dataDxfId="2"/>
+    <tableColumn id="26" name="Colonne22" dataDxfId="1"/>
+    <tableColumn id="27" name="Colonne23" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2041,11 +2045,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U35" sqref="A35:U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -3484,8 +3488,21 @@
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="16" t="n"/>
-      <c r="C35" s="16" t="n"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Clement</t>
+        </is>
+      </c>
+      <c r="B35" s="16" t="inlineStr">
+        <is>
+          <t>11'34</t>
+        </is>
+      </c>
+      <c r="C35" s="16" t="inlineStr">
+        <is>
+          <t>24'15</t>
+        </is>
+      </c>
       <c r="D35" s="16" t="n"/>
       <c r="E35" s="16" t="n"/>
       <c r="F35" s="16" t="n"/>
@@ -3494,7 +3511,11 @@
       <c r="I35" s="16" t="n"/>
       <c r="J35" s="16" t="n"/>
       <c r="K35" s="16" t="n"/>
-      <c r="L35" s="16" t="n"/>
+      <c r="L35" s="16" t="inlineStr">
+        <is>
+          <t>5m44</t>
+        </is>
+      </c>
       <c r="M35" s="16" t="n"/>
       <c r="N35" s="16" t="n"/>
       <c r="O35" s="16" t="n"/>
@@ -3504,8 +3525,21 @@
       <c r="S35" s="16" t="n"/>
     </row>
     <row r="36">
-      <c r="B36" s="16" t="n"/>
-      <c r="C36" s="16" t="n"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Tom</t>
+        </is>
+      </c>
+      <c r="B36" s="16" t="inlineStr">
+        <is>
+          <t>11'44</t>
+        </is>
+      </c>
+      <c r="C36" s="16" t="inlineStr">
+        <is>
+          <t>23'96</t>
+        </is>
+      </c>
       <c r="D36" s="16" t="n"/>
       <c r="E36" s="16" t="n"/>
       <c r="F36" s="16" t="n"/>
@@ -3514,7 +3548,11 @@
       <c r="I36" s="16" t="n"/>
       <c r="J36" s="16" t="n"/>
       <c r="K36" s="16" t="n"/>
-      <c r="L36" s="16" t="n"/>
+      <c r="L36" s="16" t="inlineStr">
+        <is>
+          <t>5m58</t>
+        </is>
+      </c>
       <c r="M36" s="16" t="n"/>
       <c r="N36" s="16" t="n"/>
       <c r="O36" s="16" t="n"/>
@@ -3524,8 +3562,21 @@
       <c r="S36" s="16" t="n"/>
     </row>
     <row r="37">
-      <c r="B37" s="16" t="n"/>
-      <c r="C37" s="16" t="n"/>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Yann</t>
+        </is>
+      </c>
+      <c r="B37" s="16" t="inlineStr">
+        <is>
+          <t>11'81</t>
+        </is>
+      </c>
+      <c r="C37" s="16" t="inlineStr">
+        <is>
+          <t>26'50</t>
+        </is>
+      </c>
       <c r="D37" s="16" t="n"/>
       <c r="E37" s="16" t="n"/>
       <c r="F37" s="16" t="n"/>
@@ -3534,35 +3585,175 @@
       <c r="I37" s="16" t="n"/>
       <c r="J37" s="16" t="n"/>
       <c r="K37" s="16" t="n"/>
-      <c r="L37" s="16" t="n"/>
+      <c r="L37" s="16" t="inlineStr">
+        <is>
+          <t>4m70</t>
+        </is>
+      </c>
       <c r="M37" s="16" t="n"/>
-      <c r="N37" s="16" t="n"/>
+      <c r="N37" s="16" t="inlineStr">
+        <is>
+          <t>8m89</t>
+        </is>
+      </c>
       <c r="O37" s="16" t="n"/>
       <c r="P37" s="16" t="n"/>
-      <c r="Q37" s="16" t="n"/>
+      <c r="Q37" s="16" t="inlineStr">
+        <is>
+          <t>16m65</t>
+        </is>
+      </c>
       <c r="R37" s="16" t="n"/>
       <c r="S37" s="16" t="n"/>
     </row>
     <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Leo</t>
+        </is>
+      </c>
       <c r="B38" s="16" t="n"/>
-      <c r="C38" s="16" t="n"/>
-      <c r="D38" s="16" t="n"/>
-      <c r="E38" s="16" t="n"/>
-      <c r="F38" s="16" t="n"/>
+      <c r="C38" s="16" t="inlineStr">
+        <is>
+          <t>23'89</t>
+        </is>
+      </c>
+      <c r="D38" s="16" t="inlineStr">
+        <is>
+          <t>51'15</t>
+        </is>
+      </c>
+      <c r="E38" s="16" t="inlineStr">
+        <is>
+          <t>1'55'16</t>
+        </is>
+      </c>
+      <c r="F38" s="16" t="inlineStr">
+        <is>
+          <t>4'03'17</t>
+        </is>
+      </c>
       <c r="G38" s="16" t="n"/>
       <c r="H38" s="16" t="n"/>
       <c r="I38" s="16" t="n"/>
-      <c r="J38" s="16" t="n"/>
+      <c r="J38" s="16" t="inlineStr">
+        <is>
+          <t>60'63</t>
+        </is>
+      </c>
       <c r="K38" s="16" t="n"/>
       <c r="L38" s="16" t="n"/>
       <c r="M38" s="16" t="n"/>
       <c r="N38" s="16" t="n"/>
       <c r="O38" s="16" t="n"/>
       <c r="P38" s="16" t="n"/>
-      <c r="Q38" s="16" t="n"/>
+      <c r="Q38" s="16" t="inlineStr">
+        <is>
+          <t>26m77</t>
+        </is>
+      </c>
       <c r="R38" s="16" t="n"/>
       <c r="S38" s="16" t="n"/>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Bryan</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11'96</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>24'19</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>51'54</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>1'58'33</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>59'02</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>5m24</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>4m66</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Gaetan</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>24'44</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>54'12</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>4m94</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Geoffrey</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>23'09</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>53'22</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Gwen</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>31'07'02</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>1m40</t>
+        </is>
+      </c>
+    </row>
+    <row r="43"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
@@ -3578,11 +3769,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:R1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="A32:O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -4637,6 +4828,189 @@
       </c>
       <c r="S31" s="16" t="n"/>
       <c r="T31" s="16" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Yuna</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>12'29</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>24'72</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>5m09</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>12'83</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>26'34</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>57'48</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2'18'30</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>70'52</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>3m90</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>12m06</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>13'00</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>26'98</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>3m88</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>7m45</t>
+        </is>
+      </c>
+    </row>
+    <row r="35"/>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Yuna</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>12'29</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>24'72</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>5m09</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>12'83</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>26'34</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>57'48</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2'18'30</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>70'52</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>3m90</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>12m06</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>13'00</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>26'98</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>3m88</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>7m45</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16375,8 +16749,8 @@
   </sheetPr>
   <dimension ref="A1:AS250"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -16407,7 +16781,7 @@
       </c>
       <c r="E1" s="32" t="inlineStr">
         <is>
-          <t>Colonne1</t>
+          <t>Alias</t>
         </is>
       </c>
       <c r="F1" s="33" t="inlineStr">
@@ -16513,6 +16887,11 @@
       <c r="Z1" s="34" t="inlineStr">
         <is>
           <t>Colonne22</t>
+        </is>
+      </c>
+      <c r="AA1" s="30" t="inlineStr">
+        <is>
+          <t>Colonne23</t>
         </is>
       </c>
     </row>
@@ -16537,15 +16916,19 @@
       </c>
       <c r="E2" s="16" t="inlineStr">
         <is>
+          <t>Clement</t>
+        </is>
+      </c>
+      <c r="F2" s="16" t="inlineStr">
+        <is>
           <t>11'34</t>
         </is>
       </c>
-      <c r="F2" s="16" t="inlineStr">
+      <c r="G2" s="16" t="inlineStr">
         <is>
           <t>24'15</t>
         </is>
       </c>
-      <c r="G2" s="16" t="inlineStr"/>
       <c r="H2" s="16" t="inlineStr"/>
       <c r="I2" s="16" t="inlineStr"/>
       <c r="J2" s="16" t="inlineStr"/>
@@ -16553,19 +16936,19 @@
       <c r="L2" s="16" t="inlineStr"/>
       <c r="M2" s="16" t="inlineStr"/>
       <c r="N2" s="16" t="inlineStr"/>
-      <c r="O2" s="16" t="inlineStr">
+      <c r="O2" s="16" t="inlineStr"/>
+      <c r="P2" s="16" t="inlineStr">
         <is>
           <t>5m44</t>
         </is>
       </c>
-      <c r="P2" s="16" t="inlineStr"/>
       <c r="Q2" s="16" t="inlineStr"/>
       <c r="R2" s="16" t="inlineStr"/>
       <c r="S2" s="16" t="inlineStr"/>
       <c r="T2" s="16" t="inlineStr"/>
       <c r="U2" s="16" t="inlineStr"/>
       <c r="V2" s="16" t="inlineStr"/>
-      <c r="W2" s="16" t="n"/>
+      <c r="W2" s="16" t="inlineStr"/>
       <c r="X2" s="16" t="n"/>
       <c r="Y2" s="16" t="n"/>
       <c r="Z2" s="16" t="n"/>
@@ -16608,15 +16991,19 @@
       </c>
       <c r="E3" s="16" t="inlineStr">
         <is>
+          <t>Tom</t>
+        </is>
+      </c>
+      <c r="F3" s="16" t="inlineStr">
+        <is>
           <t>11'44</t>
         </is>
       </c>
-      <c r="F3" s="16" t="inlineStr">
+      <c r="G3" s="16" t="inlineStr">
         <is>
           <t>23'96</t>
         </is>
       </c>
-      <c r="G3" s="16" t="inlineStr"/>
       <c r="H3" s="16" t="inlineStr"/>
       <c r="I3" s="16" t="inlineStr"/>
       <c r="J3" s="16" t="inlineStr"/>
@@ -16624,19 +17011,19 @@
       <c r="L3" s="16" t="inlineStr"/>
       <c r="M3" s="16" t="inlineStr"/>
       <c r="N3" s="16" t="inlineStr"/>
-      <c r="O3" s="16" t="inlineStr">
+      <c r="O3" s="16" t="inlineStr"/>
+      <c r="P3" s="16" t="inlineStr">
         <is>
           <t>5m58</t>
         </is>
       </c>
-      <c r="P3" s="16" t="inlineStr"/>
       <c r="Q3" s="16" t="inlineStr"/>
       <c r="R3" s="16" t="inlineStr"/>
       <c r="S3" s="16" t="inlineStr"/>
       <c r="T3" s="16" t="inlineStr"/>
       <c r="U3" s="16" t="inlineStr"/>
       <c r="V3" s="16" t="inlineStr"/>
-      <c r="W3" s="16" t="n"/>
+      <c r="W3" s="16" t="inlineStr"/>
       <c r="X3" s="16" t="n"/>
       <c r="Y3" s="16" t="n"/>
       <c r="Z3" s="16" t="n"/>
@@ -16679,15 +17066,19 @@
       </c>
       <c r="E4" s="16" t="inlineStr">
         <is>
+          <t>Yann</t>
+        </is>
+      </c>
+      <c r="F4" s="16" t="inlineStr">
+        <is>
           <t>11'81</t>
         </is>
       </c>
-      <c r="F4" s="16" t="inlineStr">
+      <c r="G4" s="16" t="inlineStr">
         <is>
           <t>26'50</t>
         </is>
       </c>
-      <c r="G4" s="16" t="inlineStr"/>
       <c r="H4" s="16" t="inlineStr"/>
       <c r="I4" s="16" t="inlineStr"/>
       <c r="J4" s="16" t="inlineStr"/>
@@ -16695,27 +17086,27 @@
       <c r="L4" s="16" t="inlineStr"/>
       <c r="M4" s="16" t="inlineStr"/>
       <c r="N4" s="16" t="inlineStr"/>
-      <c r="O4" s="16" t="inlineStr">
+      <c r="O4" s="16" t="inlineStr"/>
+      <c r="P4" s="16" t="inlineStr">
         <is>
           <t>4m70</t>
         </is>
       </c>
-      <c r="P4" s="16" t="inlineStr"/>
-      <c r="Q4" s="16" t="inlineStr">
+      <c r="Q4" s="16" t="inlineStr"/>
+      <c r="R4" s="16" t="inlineStr">
         <is>
           <t>8m89</t>
         </is>
       </c>
-      <c r="R4" s="16" t="inlineStr"/>
       <c r="S4" s="16" t="inlineStr"/>
-      <c r="T4" s="16" t="inlineStr">
+      <c r="T4" s="16" t="inlineStr"/>
+      <c r="U4" s="16" t="inlineStr">
         <is>
           <t>16m65</t>
         </is>
       </c>
-      <c r="U4" s="16" t="inlineStr"/>
       <c r="V4" s="16" t="inlineStr"/>
-      <c r="W4" s="16" t="n"/>
+      <c r="W4" s="16" t="inlineStr"/>
       <c r="X4" s="16" t="n"/>
       <c r="Y4" s="16" t="n"/>
       <c r="Z4" s="16" t="n"/>
@@ -16756,49 +17147,53 @@
           <t>M</t>
         </is>
       </c>
-      <c r="E5" s="16" t="inlineStr"/>
-      <c r="F5" s="16" t="inlineStr">
+      <c r="E5" s="16" t="inlineStr">
+        <is>
+          <t>Leo</t>
+        </is>
+      </c>
+      <c r="F5" s="16" t="inlineStr"/>
+      <c r="G5" s="16" t="inlineStr">
         <is>
           <t>23'89</t>
         </is>
       </c>
-      <c r="G5" s="16" t="inlineStr">
+      <c r="H5" s="16" t="inlineStr">
         <is>
           <t>51'15</t>
         </is>
       </c>
-      <c r="H5" s="16" t="inlineStr">
+      <c r="I5" s="16" t="inlineStr">
         <is>
           <t>1'55'16</t>
         </is>
       </c>
-      <c r="I5" s="16" t="inlineStr">
+      <c r="J5" s="16" t="inlineStr">
         <is>
           <t>4'03'17</t>
         </is>
       </c>
-      <c r="J5" s="16" t="inlineStr"/>
       <c r="K5" s="16" t="inlineStr"/>
       <c r="L5" s="16" t="inlineStr"/>
-      <c r="M5" s="16" t="inlineStr">
+      <c r="M5" s="16" t="inlineStr"/>
+      <c r="N5" s="16" t="inlineStr">
         <is>
           <t>60'63</t>
         </is>
       </c>
-      <c r="N5" s="16" t="inlineStr"/>
       <c r="O5" s="16" t="inlineStr"/>
       <c r="P5" s="16" t="inlineStr"/>
       <c r="Q5" s="16" t="inlineStr"/>
       <c r="R5" s="16" t="inlineStr"/>
       <c r="S5" s="16" t="inlineStr"/>
-      <c r="T5" s="16" t="inlineStr">
+      <c r="T5" s="16" t="inlineStr"/>
+      <c r="U5" s="16" t="inlineStr">
         <is>
           <t>26m77</t>
         </is>
       </c>
-      <c r="U5" s="16" t="inlineStr"/>
       <c r="V5" s="16" t="inlineStr"/>
-      <c r="W5" s="16" t="n"/>
+      <c r="W5" s="16" t="inlineStr"/>
       <c r="X5" s="16" t="n"/>
       <c r="Y5" s="16" t="n"/>
       <c r="Z5" s="16" t="n"/>
@@ -16841,51 +17236,55 @@
       </c>
       <c r="E6" s="16" t="inlineStr">
         <is>
+          <t>Bryan</t>
+        </is>
+      </c>
+      <c r="F6" s="16" t="inlineStr">
+        <is>
           <t>11'96</t>
         </is>
       </c>
-      <c r="F6" s="16" t="inlineStr">
+      <c r="G6" s="16" t="inlineStr">
         <is>
           <t>24'19</t>
         </is>
       </c>
-      <c r="G6" s="16" t="inlineStr">
-        <is>
-          <t>51'91</t>
-        </is>
-      </c>
       <c r="H6" s="16" t="inlineStr">
         <is>
+          <t>51'54</t>
+        </is>
+      </c>
+      <c r="I6" s="16" t="inlineStr">
+        <is>
           <t>1'58'33</t>
         </is>
       </c>
-      <c r="I6" s="16" t="inlineStr"/>
       <c r="J6" s="16" t="inlineStr"/>
       <c r="K6" s="16" t="inlineStr"/>
       <c r="L6" s="16" t="inlineStr"/>
-      <c r="M6" s="16" t="inlineStr">
+      <c r="M6" s="16" t="inlineStr"/>
+      <c r="N6" s="16" t="inlineStr">
         <is>
           <t>59'02</t>
         </is>
       </c>
-      <c r="N6" s="16" t="inlineStr"/>
-      <c r="O6" s="16" t="inlineStr">
+      <c r="O6" s="16" t="inlineStr"/>
+      <c r="P6" s="16" t="inlineStr">
         <is>
           <t>5m24</t>
         </is>
       </c>
-      <c r="P6" s="16" t="inlineStr"/>
       <c r="Q6" s="16" t="inlineStr"/>
       <c r="R6" s="16" t="inlineStr"/>
-      <c r="S6" s="16" t="inlineStr">
+      <c r="S6" s="16" t="inlineStr"/>
+      <c r="T6" s="16" t="inlineStr">
         <is>
           <t>4m66</t>
         </is>
       </c>
-      <c r="T6" s="16" t="inlineStr"/>
       <c r="U6" s="16" t="inlineStr"/>
       <c r="V6" s="16" t="inlineStr"/>
-      <c r="W6" s="16" t="n"/>
+      <c r="W6" s="16" t="inlineStr"/>
       <c r="X6" s="16" t="n"/>
       <c r="Y6" s="16" t="n"/>
       <c r="Z6" s="16" t="n"/>
@@ -16926,37 +17325,41 @@
           <t>M</t>
         </is>
       </c>
-      <c r="E7" s="16" t="inlineStr"/>
-      <c r="F7" s="16" t="inlineStr">
+      <c r="E7" s="16" t="inlineStr">
+        <is>
+          <t>Gaetan</t>
+        </is>
+      </c>
+      <c r="F7" s="16" t="inlineStr"/>
+      <c r="G7" s="16" t="inlineStr">
         <is>
           <t>24'44</t>
         </is>
       </c>
-      <c r="G7" s="16" t="inlineStr">
+      <c r="H7" s="16" t="inlineStr">
         <is>
           <t>54'12</t>
         </is>
       </c>
-      <c r="H7" s="16" t="inlineStr"/>
       <c r="I7" s="16" t="inlineStr"/>
       <c r="J7" s="16" t="inlineStr"/>
       <c r="K7" s="16" t="inlineStr"/>
       <c r="L7" s="16" t="inlineStr"/>
       <c r="M7" s="16" t="inlineStr"/>
       <c r="N7" s="16" t="inlineStr"/>
-      <c r="O7" s="16" t="inlineStr">
+      <c r="O7" s="16" t="inlineStr"/>
+      <c r="P7" s="16" t="inlineStr">
         <is>
           <t>4m94</t>
         </is>
       </c>
-      <c r="P7" s="16" t="inlineStr"/>
       <c r="Q7" s="16" t="inlineStr"/>
       <c r="R7" s="16" t="inlineStr"/>
       <c r="S7" s="16" t="inlineStr"/>
       <c r="T7" s="16" t="inlineStr"/>
       <c r="U7" s="16" t="inlineStr"/>
       <c r="V7" s="16" t="inlineStr"/>
-      <c r="W7" s="16" t="n"/>
+      <c r="W7" s="16" t="inlineStr"/>
       <c r="X7" s="16" t="n"/>
       <c r="Y7" s="16" t="n"/>
       <c r="Z7" s="16" t="n"/>
@@ -16997,18 +17400,22 @@
           <t>M</t>
         </is>
       </c>
-      <c r="E8" s="16" t="inlineStr"/>
-      <c r="F8" s="16" t="inlineStr">
-        <is>
-          <t>23'10</t>
-        </is>
-      </c>
+      <c r="E8" s="16" t="inlineStr">
+        <is>
+          <t>Geoffrey</t>
+        </is>
+      </c>
+      <c r="F8" s="16" t="inlineStr"/>
       <c r="G8" s="16" t="inlineStr">
         <is>
+          <t>23'09</t>
+        </is>
+      </c>
+      <c r="H8" s="16" t="inlineStr">
+        <is>
           <t>53'22</t>
         </is>
       </c>
-      <c r="H8" s="16" t="inlineStr"/>
       <c r="I8" s="16" t="inlineStr"/>
       <c r="J8" s="16" t="inlineStr"/>
       <c r="K8" s="16" t="inlineStr"/>
@@ -17023,7 +17430,7 @@
       <c r="T8" s="16" t="inlineStr"/>
       <c r="U8" s="16" t="inlineStr"/>
       <c r="V8" s="16" t="inlineStr"/>
-      <c r="W8" s="16" t="n"/>
+      <c r="W8" s="16" t="inlineStr"/>
       <c r="X8" s="16" t="n"/>
       <c r="Y8" s="16" t="n"/>
       <c r="Z8" s="16" t="n"/>
@@ -17064,7 +17471,11 @@
           <t>M</t>
         </is>
       </c>
-      <c r="E9" s="16" t="inlineStr"/>
+      <c r="E9" s="16" t="inlineStr">
+        <is>
+          <t>Gwen</t>
+        </is>
+      </c>
       <c r="F9" s="16" t="inlineStr"/>
       <c r="G9" s="16" t="inlineStr"/>
       <c r="H9" s="16" t="inlineStr"/>
@@ -17073,24 +17484,24 @@
       <c r="K9" s="16" t="inlineStr"/>
       <c r="L9" s="16" t="inlineStr"/>
       <c r="M9" s="16" t="inlineStr"/>
-      <c r="N9" s="16" t="inlineStr">
+      <c r="N9" s="16" t="inlineStr"/>
+      <c r="O9" s="16" t="inlineStr">
         <is>
           <t>31'07'02</t>
         </is>
       </c>
-      <c r="O9" s="16" t="inlineStr"/>
-      <c r="P9" s="16" t="inlineStr">
+      <c r="P9" s="16" t="inlineStr"/>
+      <c r="Q9" s="16" t="inlineStr">
         <is>
           <t>1m40</t>
         </is>
       </c>
-      <c r="Q9" s="16" t="inlineStr"/>
       <c r="R9" s="16" t="inlineStr"/>
       <c r="S9" s="16" t="inlineStr"/>
       <c r="T9" s="16" t="inlineStr"/>
       <c r="U9" s="16" t="inlineStr"/>
       <c r="V9" s="16" t="inlineStr"/>
-      <c r="W9" s="16" t="n"/>
+      <c r="W9" s="16" t="inlineStr"/>
       <c r="X9" s="16" t="n"/>
       <c r="Y9" s="16" t="n"/>
       <c r="Z9" s="16" t="n"/>
@@ -17133,34 +17544,38 @@
       </c>
       <c r="E10" s="16" t="inlineStr">
         <is>
+          <t>Yuna</t>
+        </is>
+      </c>
+      <c r="F10" s="16" t="inlineStr">
+        <is>
           <t>12'29</t>
         </is>
       </c>
-      <c r="F10" s="16" t="inlineStr">
+      <c r="G10" s="16" t="inlineStr">
         <is>
           <t>24'72</t>
         </is>
       </c>
-      <c r="G10" s="16" t="inlineStr"/>
       <c r="H10" s="16" t="inlineStr"/>
       <c r="I10" s="16" t="inlineStr"/>
       <c r="J10" s="16" t="inlineStr"/>
       <c r="K10" s="16" t="inlineStr"/>
       <c r="L10" s="16" t="inlineStr"/>
       <c r="M10" s="16" t="inlineStr"/>
-      <c r="N10" s="16" t="inlineStr">
+      <c r="N10" s="16" t="inlineStr"/>
+      <c r="O10" s="16" t="inlineStr">
         <is>
           <t>5m09</t>
         </is>
       </c>
-      <c r="O10" s="16" t="inlineStr"/>
       <c r="P10" s="16" t="inlineStr"/>
       <c r="Q10" s="16" t="inlineStr"/>
       <c r="R10" s="16" t="inlineStr"/>
       <c r="S10" s="16" t="inlineStr"/>
       <c r="T10" s="16" t="inlineStr"/>
       <c r="U10" s="16" t="inlineStr"/>
-      <c r="V10" s="16" t="n"/>
+      <c r="V10" s="16" t="inlineStr"/>
       <c r="W10" s="16" t="n"/>
       <c r="X10" s="16" t="n"/>
       <c r="Y10" s="16" t="n"/>
@@ -17204,50 +17619,54 @@
       </c>
       <c r="E11" s="16" t="inlineStr">
         <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="F11" s="16" t="inlineStr">
+        <is>
           <t>12'83</t>
         </is>
       </c>
-      <c r="F11" s="16" t="inlineStr">
+      <c r="G11" s="16" t="inlineStr">
         <is>
           <t>26'34</t>
         </is>
       </c>
-      <c r="G11" s="16" t="inlineStr">
+      <c r="H11" s="16" t="inlineStr">
         <is>
           <t>57'48</t>
         </is>
       </c>
-      <c r="H11" s="16" t="inlineStr">
+      <c r="I11" s="16" t="inlineStr">
         <is>
           <t>2'18'30</t>
         </is>
       </c>
-      <c r="I11" s="16" t="inlineStr"/>
       <c r="J11" s="16" t="inlineStr"/>
       <c r="K11" s="16" t="inlineStr"/>
-      <c r="L11" s="16" t="inlineStr">
+      <c r="L11" s="16" t="inlineStr"/>
+      <c r="M11" s="16" t="inlineStr">
         <is>
           <t>70'52</t>
         </is>
       </c>
-      <c r="M11" s="16" t="inlineStr"/>
-      <c r="N11" s="16" t="inlineStr">
+      <c r="N11" s="16" t="inlineStr"/>
+      <c r="O11" s="16" t="inlineStr">
         <is>
           <t>3m90</t>
         </is>
       </c>
-      <c r="O11" s="16" t="inlineStr"/>
       <c r="P11" s="16" t="inlineStr"/>
       <c r="Q11" s="16" t="inlineStr"/>
-      <c r="R11" s="16" t="inlineStr">
+      <c r="R11" s="16" t="inlineStr"/>
+      <c r="S11" s="16" t="inlineStr">
         <is>
           <t>12m06</t>
         </is>
       </c>
-      <c r="S11" s="16" t="inlineStr"/>
       <c r="T11" s="16" t="inlineStr"/>
       <c r="U11" s="16" t="inlineStr"/>
-      <c r="V11" s="16" t="n"/>
+      <c r="V11" s="16" t="inlineStr"/>
       <c r="W11" s="16" t="n"/>
       <c r="X11" s="16" t="n"/>
       <c r="Y11" s="16" t="n"/>
@@ -17291,38 +17710,42 @@
       </c>
       <c r="E12" s="16" t="inlineStr">
         <is>
+          <t>Charlotte</t>
+        </is>
+      </c>
+      <c r="F12" s="16" t="inlineStr">
+        <is>
           <t>13'00</t>
         </is>
       </c>
-      <c r="F12" s="16" t="inlineStr">
+      <c r="G12" s="16" t="inlineStr">
         <is>
           <t>26'98</t>
         </is>
       </c>
-      <c r="G12" s="16" t="inlineStr"/>
       <c r="H12" s="16" t="inlineStr"/>
       <c r="I12" s="16" t="inlineStr"/>
       <c r="J12" s="16" t="inlineStr"/>
       <c r="K12" s="16" t="inlineStr"/>
       <c r="L12" s="16" t="inlineStr"/>
       <c r="M12" s="16" t="inlineStr"/>
-      <c r="N12" s="16" t="inlineStr">
+      <c r="N12" s="16" t="inlineStr"/>
+      <c r="O12" s="16" t="inlineStr">
         <is>
           <t>3m88</t>
         </is>
       </c>
-      <c r="O12" s="16" t="inlineStr"/>
       <c r="P12" s="16" t="inlineStr"/>
       <c r="Q12" s="16" t="inlineStr"/>
-      <c r="R12" s="16" t="inlineStr">
+      <c r="R12" s="16" t="inlineStr"/>
+      <c r="S12" s="16" t="inlineStr">
         <is>
           <t>7m45</t>
         </is>
       </c>
-      <c r="S12" s="16" t="inlineStr"/>
       <c r="T12" s="16" t="inlineStr"/>
       <c r="U12" s="16" t="inlineStr"/>
-      <c r="V12" s="16" t="n"/>
+      <c r="V12" s="16" t="inlineStr"/>
       <c r="W12" s="16" t="n"/>
       <c r="X12" s="16" t="n"/>
       <c r="Y12" s="16" t="n"/>

</xml_diff>